<commit_message>
updated the dissertation to include circle manuscript
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FFE6DC-1964-CE48-8643-2A62E4971AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF45C3A-20AA-644B-AE3B-1EE20C0285D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="1100" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
@@ -1497,8 +1497,8 @@
   <dimension ref="A1:E141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A142" sqref="A142"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1543,87 +1543,87 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>273</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>202</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>273</v>
+      <c r="A8" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="B8" t="s">
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B9" t="s">
         <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>240</v>
+      <c r="A10" t="s">
+        <v>268</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="D10" t="s">
-        <v>241</v>
+      <c r="C10" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B11" t="s">
         <v>61</v>
@@ -1634,7 +1634,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
         <v>61</v>
@@ -1645,235 +1645,232 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>271</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
-        <v>269</v>
+      <c r="D13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>265</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
       </c>
+      <c r="C14" t="s">
+        <v>266</v>
+      </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s">
-        <v>266</v>
-      </c>
       <c r="D15" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B21" t="s">
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
         <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>280</v>
       </c>
       <c r="B27" t="s">
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>206</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
-      </c>
-      <c r="D28" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>288</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>242</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>246</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
-      </c>
-      <c r="D33" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>61</v>
@@ -1881,7 +1878,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
         <v>61</v>
@@ -1889,7 +1886,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
         <v>61</v>
@@ -1897,45 +1894,45 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>254</v>
+      </c>
+      <c r="D37" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>253</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>254</v>
-      </c>
-      <c r="D38" t="s">
-        <v>255</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
         <v>61</v>
-      </c>
-      <c r="D40" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
@@ -1943,26 +1940,26 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
         <v>61</v>
-      </c>
-      <c r="D43" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
@@ -1970,7 +1967,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
         <v>61</v>
@@ -1978,111 +1975,114 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>228</v>
       </c>
       <c r="B46" t="s">
         <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>228</v>
+        <v>289</v>
       </c>
       <c r="B47" t="s">
         <v>61</v>
       </c>
       <c r="D47" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="B48" t="s">
         <v>61</v>
       </c>
       <c r="D48" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>317</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>318</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
         <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>222</v>
       </c>
       <c r="B51" t="s">
         <v>31</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>222</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
         <v>31</v>
       </c>
       <c r="D52" t="s">
-        <v>223</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>31</v>
+      </c>
+      <c r="D53" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
         <v>31</v>
       </c>
-      <c r="D54" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
         <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>262</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
         <v>31</v>
@@ -2090,285 +2090,288 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B57" t="s">
-        <v>342</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>204</v>
+        <v>340</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>258</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>259</v>
       </c>
       <c r="D58" t="s">
-        <v>79</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>337</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>259</v>
+      </c>
+      <c r="D59" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>339</v>
+        <v>251</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>342</v>
       </c>
       <c r="D60" t="s">
-        <v>340</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>258</v>
+        <v>341</v>
       </c>
       <c r="B61" t="s">
-        <v>259</v>
+        <v>342</v>
       </c>
       <c r="D61" t="s">
-        <v>260</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>337</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>259</v>
+        <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>338</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="B63" t="s">
         <v>60</v>
       </c>
+      <c r="C63" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D63" t="s">
-        <v>84</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="B64" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D64" t="s">
-        <v>173</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B65" t="s">
         <v>60</v>
-      </c>
-      <c r="D65" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="B66" t="s">
         <v>60</v>
+      </c>
+      <c r="D66" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>282</v>
+        <v>218</v>
       </c>
       <c r="B67" t="s">
         <v>60</v>
       </c>
       <c r="D67" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>5</v>
       </c>
       <c r="B68" t="s">
         <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
         <v>60</v>
       </c>
       <c r="D69" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>29</v>
+        <v>220</v>
       </c>
       <c r="B70" t="s">
         <v>60</v>
       </c>
       <c r="D70" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="B71" t="s">
         <v>60</v>
       </c>
       <c r="D71" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
       </c>
       <c r="D72" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="E72" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B73" t="s">
         <v>60</v>
       </c>
       <c r="D73" t="s">
-        <v>190</v>
-      </c>
-      <c r="E73" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="B74" t="s">
         <v>60</v>
       </c>
       <c r="D74" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B75" t="s">
         <v>60</v>
       </c>
       <c r="D75" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>196</v>
+        <v>39</v>
       </c>
       <c r="B76" t="s">
         <v>60</v>
       </c>
       <c r="D76" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B77" t="s">
         <v>60</v>
       </c>
       <c r="D77" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="B78" t="s">
         <v>60</v>
       </c>
+      <c r="C78" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D78" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B79" t="s">
         <v>60</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D79" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="B80" t="s">
         <v>60</v>
       </c>
       <c r="D80" t="s">
-        <v>205</v>
+        <v>234</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="B81" t="s">
         <v>60</v>
       </c>
       <c r="D81" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>208</v>
+        <v>275</v>
       </c>
       <c r="B82" t="s">
         <v>60</v>
@@ -2379,37 +2382,34 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>275</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>60</v>
-      </c>
-      <c r="D83" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
         <v>60</v>
+      </c>
+      <c r="D84" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B85" t="s">
         <v>60</v>
-      </c>
-      <c r="D85" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
         <v>60</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B87" t="s">
         <v>60</v>
@@ -2425,26 +2425,26 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>244</v>
       </c>
       <c r="B88" t="s">
         <v>60</v>
+      </c>
+      <c r="D88" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
         <v>60</v>
-      </c>
-      <c r="D89" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B90" t="s">
         <v>60</v>
@@ -2452,56 +2452,56 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
         <v>60</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>2</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>3</v>
+      <c r="D92" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>248</v>
+        <v>87</v>
       </c>
       <c r="B93" t="s">
         <v>60</v>
-      </c>
-      <c r="D93" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>87</v>
+        <v>256</v>
       </c>
       <c r="B94" t="s">
         <v>60</v>
+      </c>
+      <c r="D94" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>256</v>
+        <v>44</v>
       </c>
       <c r="B95" t="s">
         <v>60</v>
-      </c>
-      <c r="D95" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
         <v>60</v>
@@ -2509,26 +2509,26 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B97" t="s">
         <v>60</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
         <v>60</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
         <v>60</v>
@@ -2536,330 +2536,330 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="B100" t="s">
         <v>60</v>
+      </c>
+      <c r="D100" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
       <c r="B101" t="s">
         <v>60</v>
       </c>
       <c r="D101" t="s">
-        <v>36</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>210</v>
+        <v>293</v>
       </c>
       <c r="B102" t="s">
         <v>60</v>
       </c>
       <c r="D102" t="s">
-        <v>211</v>
+        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B103" t="s">
         <v>60</v>
       </c>
       <c r="D103" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B104" t="s">
         <v>60</v>
       </c>
       <c r="D104" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B105" t="s">
         <v>60</v>
       </c>
       <c r="D105" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B106" t="s">
         <v>60</v>
       </c>
       <c r="D106" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B107" t="s">
         <v>60</v>
       </c>
       <c r="D107" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B108" t="s">
         <v>60</v>
       </c>
       <c r="D108" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B109" t="s">
         <v>60</v>
       </c>
       <c r="D109" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B110" t="s">
         <v>60</v>
       </c>
       <c r="D110" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B111" t="s">
         <v>60</v>
       </c>
       <c r="D111" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B112" t="s">
         <v>60</v>
       </c>
       <c r="D112" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B113" t="s">
         <v>60</v>
       </c>
       <c r="D113" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B114" t="s">
         <v>60</v>
       </c>
       <c r="D114" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B115" t="s">
         <v>60</v>
       </c>
       <c r="D115" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B116" t="s">
         <v>60</v>
       </c>
       <c r="D116" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B117" t="s">
         <v>60</v>
       </c>
       <c r="D117" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B118" t="s">
         <v>60</v>
       </c>
       <c r="D118" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>333</v>
-      </c>
-      <c r="B119" t="s">
-        <v>60</v>
-      </c>
-      <c r="D119" t="s">
-        <v>334</v>
-      </c>
+      <c r="A119" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B120" s="5" t="s">
+      <c r="A120" t="s">
+        <v>278</v>
+      </c>
+      <c r="B120" t="s">
         <v>62</v>
       </c>
-      <c r="C120" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D120" s="1"/>
+      <c r="D120" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>278</v>
+        <v>21</v>
       </c>
       <c r="B121" t="s">
         <v>62</v>
       </c>
       <c r="D121" t="s">
-        <v>279</v>
+        <v>182</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="B122" t="s">
         <v>62</v>
       </c>
+      <c r="C122" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D122" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>180</v>
+        <v>276</v>
       </c>
       <c r="B123" t="s">
         <v>62</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D123" t="s">
-        <v>188</v>
+        <v>277</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>276</v>
+        <v>86</v>
       </c>
       <c r="B124" t="s">
         <v>62</v>
       </c>
-      <c r="D124" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="B125" t="s">
         <v>62</v>
       </c>
+      <c r="D125" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B126" t="s">
         <v>62</v>
       </c>
       <c r="D126" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>27</v>
+        <v>291</v>
       </c>
       <c r="B127" t="s">
         <v>62</v>
       </c>
       <c r="D127" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="B128" t="s">
         <v>62</v>
       </c>
       <c r="D128" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>311</v>
+        <v>56</v>
       </c>
       <c r="B129" t="s">
-        <v>62</v>
-      </c>
-      <c r="D129" t="s">
-        <v>312</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2956,8 +2956,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E140">
-    <sortCondition ref="B2:B140"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E141">
+    <sortCondition ref="B2:B141"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished intro of chapter 3
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF45C3A-20AA-644B-AE3B-1EE20C0285D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0CB1A-1A0E-0A4E-83CB-8F6018632E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1100" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="15080" yWindow="500" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="360">
   <si>
     <t>Paper</t>
   </si>
@@ -1094,6 +1094,51 @@
   </si>
   <si>
     <t>The attraction effect in experience-based decisions</t>
+  </si>
+  <si>
+    <t>Finn &amp; Louviere 1992</t>
+  </si>
+  <si>
+    <t>original best-worst choice paper</t>
+  </si>
+  <si>
+    <t>best-worst scaling healthcare</t>
+  </si>
+  <si>
+    <t>Cheung et al 2016</t>
+  </si>
+  <si>
+    <t>Best–worst scaling: What it can do for health care research and how to do it</t>
+  </si>
+  <si>
+    <t>Flynn et al 2007</t>
+  </si>
+  <si>
+    <t>best worst choice in transportation</t>
+  </si>
+  <si>
+    <t>Hausman &amp; McFadden 1984</t>
+  </si>
+  <si>
+    <t>multinomal logit cite</t>
+  </si>
+  <si>
+    <t>marley 2008</t>
+  </si>
+  <si>
+    <t>check on other authors, but set dependent bw choice</t>
+  </si>
+  <si>
+    <t>marley 2012</t>
+  </si>
+  <si>
+    <t>check on other authors, but multi attribute bw choice</t>
+  </si>
+  <si>
+    <t>flynn 2014</t>
+  </si>
+  <si>
+    <t>check on other authors, but bw choice review in handbook</t>
   </si>
 </sst>
 </file>
@@ -1494,11 +1539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2905,59 +2950,118 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>213</v>
+        <v>214</v>
+      </c>
+      <c r="D134" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>214</v>
-      </c>
-      <c r="D135" t="s">
-        <v>215</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>237</v>
+        <v>287</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>287</v>
+        <v>327</v>
+      </c>
+      <c r="D138" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="D139" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="D140" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D141" t="s">
-        <v>344</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>348</v>
+      </c>
+      <c r="D142" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>350</v>
+      </c>
+      <c r="D143" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>213</v>
+      </c>
+      <c r="D144" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>352</v>
+      </c>
+      <c r="D145" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>354</v>
+      </c>
+      <c r="D146" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>356</v>
+      </c>
+      <c r="D147" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>358</v>
+      </c>
+      <c r="D148" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E141">
-    <sortCondition ref="B2:B141"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E140">
+    <sortCondition ref="B2:B140"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
split into separate tex files for each chapter
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0CB1A-1A0E-0A4E-83CB-8F6018632E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F6751E-C3F9-614F-848E-0097B228DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="500" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="15920" yWindow="500" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="364">
   <si>
     <t>Paper</t>
   </si>
@@ -1139,6 +1139,18 @@
   </si>
   <si>
     <t>check on other authors, but bw choice review in handbook</t>
+  </si>
+  <si>
+    <t>Miller et al 2011</t>
+  </si>
+  <si>
+    <t>Important paper on comparison of wtp, suggests open ended responses is fine</t>
+  </si>
+  <si>
+    <t>another wtp review</t>
+  </si>
+  <si>
+    <t>Schmidt and Bijmoldt 2020</t>
   </si>
 </sst>
 </file>
@@ -1539,11 +1551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
+      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3057,6 +3069,22 @@
       </c>
       <c r="D148" t="s">
         <v>359</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>360</v>
+      </c>
+      <c r="D149" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>363</v>
+      </c>
+      <c r="D150" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got a lot of work done 5/12
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F6751E-C3F9-614F-848E-0097B228DA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0195A6B6-21E4-1243-800A-7D3C81906577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="500" windowWidth="27200" windowHeight="15000" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="9000" yWindow="500" windowWidth="28800" windowHeight="15860" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="381">
   <si>
     <t>Paper</t>
   </si>
@@ -1151,6 +1151,57 @@
   </si>
   <si>
     <t>Schmidt and Bijmoldt 2020</t>
+  </si>
+  <si>
+    <t>bayesian model of CE in value-based choice</t>
+  </si>
+  <si>
+    <t>Context Dependence and Aggregation in Disaggregate Choice Analysis</t>
+  </si>
+  <si>
+    <t>range-normalization model</t>
+  </si>
+  <si>
+    <t>CE choice model</t>
+  </si>
+  <si>
+    <t>mlba</t>
+  </si>
+  <si>
+    <t>review - Theories of context effects in multialternative, multiattribute choice</t>
+  </si>
+  <si>
+    <t>mlca</t>
+  </si>
+  <si>
+    <t>2n ary choice tree</t>
+  </si>
+  <si>
+    <t>Stochastic choice: An optimizing neuroeconomic model</t>
+  </si>
+  <si>
+    <t>Testing the effect of time pressure on asymmetric dominance and compromise decoys in choice</t>
+  </si>
+  <si>
+    <t>Pettibone 2000</t>
+  </si>
+  <si>
+    <t>Examining {Models} of {Nondominated} {Decoy} {Effects} across {Judgment} and {Choice}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact of choice set complexity on decoy effects, also eye-tracking and comparison </t>
+  </si>
+  <si>
+    <t>Wedell &amp; Pettibone 1996</t>
+  </si>
+  <si>
+    <t>Using Judgments to Understand Decoy Effects in Choice</t>
+  </si>
+  <si>
+    <t>Windschitl &amp; Chambers 2004</t>
+  </si>
+  <si>
+    <t>The Dud-Alternative Effect in Likelihood Judgment</t>
   </si>
 </sst>
 </file>
@@ -1551,11 +1602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1924,6 +1975,9 @@
       <c r="B33" t="s">
         <v>61</v>
       </c>
+      <c r="D33" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1940,6 +1994,9 @@
       <c r="B35" t="s">
         <v>61</v>
       </c>
+      <c r="D35" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1948,6 +2005,9 @@
       <c r="B36" t="s">
         <v>61</v>
       </c>
+      <c r="D36" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1967,6 +2027,9 @@
       <c r="B38" t="s">
         <v>61</v>
       </c>
+      <c r="D38" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1986,6 +2049,9 @@
       <c r="B40" t="s">
         <v>61</v>
       </c>
+      <c r="D40" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1994,6 +2060,9 @@
       <c r="B41" t="s">
         <v>61</v>
       </c>
+      <c r="D41" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2013,6 +2082,9 @@
       <c r="B43" t="s">
         <v>61</v>
       </c>
+      <c r="D43" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -2021,6 +2093,9 @@
       <c r="B44" t="s">
         <v>61</v>
       </c>
+      <c r="D44" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2029,6 +2104,9 @@
       <c r="B45" t="s">
         <v>61</v>
       </c>
+      <c r="D45" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -2479,6 +2557,9 @@
       <c r="B87" t="s">
         <v>60</v>
       </c>
+      <c r="D87" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -2536,6 +2617,9 @@
       <c r="B93" t="s">
         <v>60</v>
       </c>
+      <c r="D93" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -3085,6 +3169,30 @@
       </c>
       <c r="D150" t="s">
         <v>362</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>374</v>
+      </c>
+      <c r="D151" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>377</v>
+      </c>
+      <c r="D152" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>379</v>
+      </c>
+      <c r="D153" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now i'm done for the day 5/16
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98694D0B-0785-0143-83CE-DCE7FF2FA699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC4C1E-E8C2-1B45-BC2C-2743C614E00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="1000" windowWidth="28800" windowHeight="15860" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="11880" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="393">
   <si>
     <t>Paper</t>
   </si>
@@ -1222,6 +1222,28 @@
     <t>The timescale and direction of influence of
 a third inferior alternative in human value-
 learning</t>
+  </si>
+  <si>
+    <t>Louviere et al 2008</t>
+  </si>
+  <si>
+    <t>Modeling the choices of individual
+decision-makers by combining efficient choice
+experiment designs with extra preference
+information</t>
+  </si>
+  <si>
+    <t>Gerzinic et al 2021</t>
+  </si>
+  <si>
+    <t>Estimating decision rule differences between ‘best’ and ‘worst’
+choices in a sequential best worst discrete choice experiment</t>
+  </si>
+  <si>
+    <t>Flynn 2010</t>
+  </si>
+  <si>
+    <t>Valuing citizen and patient preferences in health: recent developments in three types of best–worst scaling</t>
   </si>
 </sst>
 </file>
@@ -1622,11 +1644,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D156" sqref="D156"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3234,6 +3256,30 @@
       </c>
       <c r="D156" t="s">
         <v>386</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>387</v>
+      </c>
+      <c r="D157" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>389</v>
+      </c>
+      <c r="D158" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>391</v>
+      </c>
+      <c r="D159" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done working for now 5/20
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC4C1E-E8C2-1B45-BC2C-2743C614E00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A2296-55F4-0641-8A86-506C4ADB8FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="9080" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="395">
   <si>
     <t>Paper</t>
   </si>
@@ -1244,6 +1244,12 @@
   </si>
   <si>
     <t>Valuing citizen and patient preferences in health: recent developments in three types of best–worst scaling</t>
+  </si>
+  <si>
+    <t>Hawkins et al 2019</t>
+  </si>
+  <si>
+    <t>common value representation for best and worst choice</t>
   </si>
 </sst>
 </file>
@@ -1644,11 +1650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
+      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3280,6 +3286,14 @@
       </c>
       <c r="D159" t="s">
         <v>392</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>393</v>
+      </c>
+      <c r="D160" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done for the day 5/28
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A2296-55F4-0641-8A86-506C4ADB8FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8D327C-A0AF-7942-B3F7-DDE56AA138C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="3480" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="400">
   <si>
     <t>Paper</t>
   </si>
@@ -1250,6 +1250,21 @@
   </si>
   <si>
     <t>common value representation for best and worst choice</t>
+  </si>
+  <si>
+    <t>MDF stuff</t>
+  </si>
+  <si>
+    <t>state-trace analysis</t>
+  </si>
+  <si>
+    <t>Teodorescu &amp; Usher 2013</t>
+  </si>
+  <si>
+    <t>Macho &amp; Ledermann 2022</t>
+  </si>
+  <si>
+    <t>A psychometric analysis of signal detection measures from ratings versus repeated and nonrepeated forced choices.</t>
   </si>
 </sst>
 </file>
@@ -1650,17 +1665,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C171AFE-CCE2-6C44-98C1-AE74A126A934}">
-  <dimension ref="A1:E160"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D160" sqref="D160"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="0" style="1" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3085,6 +3100,9 @@
       <c r="A133" t="s">
         <v>214</v>
       </c>
+      <c r="B133" t="s">
+        <v>61</v>
+      </c>
       <c r="D133" t="s">
         <v>215</v>
       </c>
@@ -3093,11 +3111,23 @@
       <c r="A134" t="s">
         <v>284</v>
       </c>
+      <c r="B134" t="s">
+        <v>61</v>
+      </c>
+      <c r="D134" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>237</v>
       </c>
+      <c r="B135" t="s">
+        <v>61</v>
+      </c>
+      <c r="D135" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -3294,6 +3324,19 @@
       </c>
       <c r="D160" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>398</v>
+      </c>
+      <c r="D162" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full draft done. Proofreading tomorrow then sending to committee. 7/9/25
</commit_message>
<xml_diff>
--- a/dissertation_lit.xlsx
+++ b/dissertation_lit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanconway/Research/Dissertation/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8D327C-A0AF-7942-B3F7-DDE56AA138C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79B7E2A-03EC-8944-9EDA-AF5EFCE2CC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{54695D73-491C-3E44-ACFD-E202721A2B0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -954,9 +954,6 @@
 the role of induced cognitive reflection</t>
   </si>
   <si>
-    <t>Pan et al 1995</t>
-  </si>
-  <si>
     <t>The attraction effect and political choice in two elections.</t>
   </si>
   <si>
@@ -1265,6 +1262,9 @@
   </si>
   <si>
     <t>A psychometric analysis of signal detection measures from ratings versus repeated and nonrepeated forced choices.</t>
+  </si>
+  <si>
+    <t>O'curry &amp; Pitts 1995</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,7 +2028,7 @@
         <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2047,7 +2047,7 @@
         <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2058,7 +2058,7 @@
         <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2080,7 +2080,7 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2102,7 +2102,7 @@
         <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2113,7 +2113,7 @@
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2135,7 +2135,7 @@
         <v>61</v>
       </c>
       <c r="D42" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -2157,7 +2157,7 @@
         <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2184,13 +2184,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>314</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" t="s">
         <v>315</v>
-      </c>
-      <c r="B47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2277,13 +2277,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B56" t="s">
         <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2299,13 +2299,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B58" t="s">
         <v>257</v>
       </c>
       <c r="D58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
         <v>249</v>
       </c>
       <c r="B59" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D59" t="s">
         <v>250</v>
@@ -2321,10 +2321,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>338</v>
+      </c>
+      <c r="B60" t="s">
         <v>339</v>
-      </c>
-      <c r="B60" t="s">
-        <v>340</v>
       </c>
       <c r="D60" t="s">
         <v>204</v>
@@ -2610,7 +2610,7 @@
         <v>60</v>
       </c>
       <c r="D86" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2670,7 +2670,7 @@
         <v>60</v>
       </c>
       <c r="D92" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2806,134 +2806,134 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>399</v>
+      </c>
+      <c r="B106" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" t="s">
         <v>301</v>
-      </c>
-      <c r="B106" t="s">
-        <v>60</v>
-      </c>
-      <c r="D106" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>302</v>
+      </c>
+      <c r="B107" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" t="s">
         <v>303</v>
-      </c>
-      <c r="B107" t="s">
-        <v>60</v>
-      </c>
-      <c r="D107" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>304</v>
+      </c>
+      <c r="B108" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108" t="s">
         <v>305</v>
-      </c>
-      <c r="B108" t="s">
-        <v>60</v>
-      </c>
-      <c r="D108" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>306</v>
+      </c>
+      <c r="B109" t="s">
+        <v>60</v>
+      </c>
+      <c r="D109" t="s">
         <v>307</v>
-      </c>
-      <c r="B109" t="s">
-        <v>60</v>
-      </c>
-      <c r="D109" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>310</v>
+      </c>
+      <c r="B110" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" t="s">
         <v>311</v>
-      </c>
-      <c r="B110" t="s">
-        <v>60</v>
-      </c>
-      <c r="D110" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>312</v>
+      </c>
+      <c r="B111" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" t="s">
         <v>313</v>
-      </c>
-      <c r="B111" t="s">
-        <v>60</v>
-      </c>
-      <c r="D111" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>316</v>
+      </c>
+      <c r="B112" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" t="s">
         <v>317</v>
-      </c>
-      <c r="B112" t="s">
-        <v>60</v>
-      </c>
-      <c r="D112" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>318</v>
+      </c>
+      <c r="B113" t="s">
+        <v>60</v>
+      </c>
+      <c r="D113" t="s">
         <v>319</v>
-      </c>
-      <c r="B113" t="s">
-        <v>60</v>
-      </c>
-      <c r="D113" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" t="s">
+        <v>60</v>
+      </c>
+      <c r="D114" t="s">
         <v>323</v>
-      </c>
-      <c r="B114" t="s">
-        <v>60</v>
-      </c>
-      <c r="D114" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>326</v>
+      </c>
+      <c r="B115" t="s">
+        <v>60</v>
+      </c>
+      <c r="D115" t="s">
         <v>327</v>
-      </c>
-      <c r="B115" t="s">
-        <v>60</v>
-      </c>
-      <c r="D115" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>328</v>
+      </c>
+      <c r="B116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D116" t="s">
         <v>329</v>
-      </c>
-      <c r="B116" t="s">
-        <v>60</v>
-      </c>
-      <c r="D116" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>330</v>
+      </c>
+      <c r="B117" t="s">
+        <v>60</v>
+      </c>
+      <c r="D117" t="s">
         <v>331</v>
-      </c>
-      <c r="B117" t="s">
-        <v>60</v>
-      </c>
-      <c r="D117" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3038,13 +3038,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B127" t="s">
         <v>62</v>
       </c>
       <c r="D127" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -3087,13 +3087,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B132" t="s">
         <v>88</v>
       </c>
       <c r="D132" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -3115,7 +3115,7 @@
         <v>61</v>
       </c>
       <c r="D134" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3126,7 +3126,7 @@
         <v>61</v>
       </c>
       <c r="D135" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3136,50 +3136,50 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>324</v>
+      </c>
+      <c r="D137" t="s">
         <v>325</v>
-      </c>
-      <c r="D137" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>332</v>
+      </c>
+      <c r="D138" t="s">
         <v>333</v>
-      </c>
-      <c r="D138" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>340</v>
+      </c>
+      <c r="D139" t="s">
         <v>341</v>
-      </c>
-      <c r="D139" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>342</v>
+      </c>
+      <c r="D140" t="s">
         <v>343</v>
-      </c>
-      <c r="D140" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D141" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D142" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3187,156 +3187,156 @@
         <v>213</v>
       </c>
       <c r="D143" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>349</v>
+      </c>
+      <c r="D144" t="s">
         <v>350</v>
-      </c>
-      <c r="D144" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>351</v>
+      </c>
+      <c r="D145" t="s">
         <v>352</v>
-      </c>
-      <c r="D145" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>353</v>
+      </c>
+      <c r="D146" t="s">
         <v>354</v>
-      </c>
-      <c r="D146" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>355</v>
+      </c>
+      <c r="D147" t="s">
         <v>356</v>
-      </c>
-      <c r="D147" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>357</v>
+      </c>
+      <c r="D148" t="s">
         <v>358</v>
-      </c>
-      <c r="D148" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D149" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>371</v>
+      </c>
+      <c r="D150" t="s">
         <v>372</v>
-      </c>
-      <c r="D150" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>374</v>
+      </c>
+      <c r="D151" t="s">
         <v>375</v>
-      </c>
-      <c r="D151" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>376</v>
+      </c>
+      <c r="D152" t="s">
         <v>377</v>
-      </c>
-      <c r="D152" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>378</v>
+      </c>
+      <c r="D153" t="s">
         <v>379</v>
-      </c>
-      <c r="D153" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>380</v>
+      </c>
+      <c r="D154" t="s">
         <v>381</v>
-      </c>
-      <c r="D154" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>382</v>
+      </c>
+      <c r="D155" t="s">
         <v>383</v>
-      </c>
-      <c r="D155" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>384</v>
+      </c>
+      <c r="D156" t="s">
         <v>385</v>
-      </c>
-      <c r="D156" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>386</v>
+      </c>
+      <c r="D157" t="s">
         <v>387</v>
-      </c>
-      <c r="D157" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>388</v>
+      </c>
+      <c r="D158" t="s">
         <v>389</v>
-      </c>
-      <c r="D158" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>390</v>
+      </c>
+      <c r="D159" t="s">
         <v>391</v>
-      </c>
-      <c r="D159" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>392</v>
+      </c>
+      <c r="D160" t="s">
         <v>393</v>
-      </c>
-      <c r="D160" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>397</v>
+      </c>
+      <c r="D162" t="s">
         <v>398</v>
-      </c>
-      <c r="D162" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>